<commit_message>
thing with potential to break program didt (due to masterful execution /s). Adding tests
</commit_message>
<xml_diff>
--- a/Tests/1/Test_SingleRun4.xlsx
+++ b/Tests/1/Test_SingleRun4.xlsx
@@ -1007,8 +1007,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A318" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,6 +1262,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="18">
+        <f>C196</f>
         <v>10</v>
       </c>
       <c r="D14" s="18"/>
@@ -1451,7 +1452,8 @@
         <v>36</v>
       </c>
       <c r="C23" s="18">
-        <v>4</v>
+        <f>C291</f>
+        <v>5</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -1471,6 +1473,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="18">
+        <f>C196</f>
         <v>10</v>
       </c>
       <c r="D24" s="17"/>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="C25">
         <f>60*C31/(C$2*(1-EXP(-1*C30*60)))</f>
-        <v>36.829070287285447</v>
+        <v>1141.1036187048715</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="17"/>
@@ -1513,7 +1516,7 @@
       </c>
       <c r="C26" s="18">
         <f>0.693/C30</f>
-        <v>13.140397230644972</v>
+        <v>1.5265676164854809</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -1533,8 +1536,8 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <f>RSQ(C297:C302,B297:B302)</f>
-        <v>1.2593842685334743E-2</v>
+        <f>RSQ(C298:C302,B298:B302)</f>
+        <v>0.97171858170986258</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="17"/>
@@ -1554,8 +1557,8 @@
         <v>26</v>
       </c>
       <c r="C28" s="18">
-        <f>SLOPE(C297:C302,B297:B302)</f>
-        <v>-2.2899753243500218E-2</v>
+        <f>SLOPE(C298:C302,B298:B302)</f>
+        <v>-0.19711662349821987</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -1575,8 +1578,8 @@
         <v>27</v>
       </c>
       <c r="C29" s="18">
-        <f>INTERCEPT(C297:C302,B297:B302)</f>
-        <v>3.0274486485223826</v>
+        <f>INTERCEPT(C298:C302,B298:B302)</f>
+        <v>4.5373281907299532</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -1597,7 +1600,7 @@
       </c>
       <c r="C30" s="18">
         <f>ABS(C28)*2.303</f>
-        <v>5.2738131719780999E-2</v>
+        <v>0.45395958391640034</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -1618,7 +1621,7 @@
       </c>
       <c r="C31" s="18">
         <f>10^C29</f>
-        <v>1065.2429006784405</v>
+        <v>34461.02499053772</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -1649,7 +1652,8 @@
         <v>37</v>
       </c>
       <c r="C33" s="18">
-        <v>4</v>
+        <f>C291</f>
+        <v>5</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1670,7 +1674,7 @@
       </c>
       <c r="C34">
         <f>60*C40/(C$2*(1-EXP(-1*C39*60)))</f>
-        <v>5077.6578935650141</v>
+        <v>19325.473306186552</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="17"/>
@@ -1691,7 +1695,7 @@
       </c>
       <c r="C35" s="18">
         <f>0.693/C39</f>
-        <v>0.63359674661589416</v>
+        <v>0.2494042704725894</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1712,7 +1716,7 @@
       </c>
       <c r="C36">
         <f>RSQ(C324:C327,B324:B327)</f>
-        <v>0.99339082280280178</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1733,7 +1737,7 @@
       </c>
       <c r="C37" s="18">
         <f>SLOPE(C324:C327,B324:B327)</f>
-        <v>-0.4749264507915244</v>
+        <v>-1.2065224606345102</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1754,7 +1758,7 @@
       </c>
       <c r="C38" s="18">
         <f>INTERCEPT(C324:C327,B324:B327)</f>
-        <v>5.1856665451084911</v>
+        <v>5.7661332472724087</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -1775,7 +1779,7 @@
       </c>
       <c r="C39" s="18">
         <f>ABS(C37)*2.303</f>
-        <v>1.0937556161728808</v>
+        <v>2.7786212268412767</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -1796,7 +1800,7 @@
       </c>
       <c r="C40" s="18">
         <f>10^C38</f>
-        <v>153343.91434355846</v>
+        <v>583624.1403872855</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -4695,7 +4699,7 @@
       </c>
       <c r="C324">
         <f t="shared" ref="C324:C326" si="6">IF(0&lt;10^C293-10^(C$28*$B324+C$29),LOG(10^C293-10^(C$28*$B324+C$29)),0)</f>
-        <v>4.7570392475239736</v>
+        <v>4.5596107866378981</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -4704,25 +4708,17 @@
       </c>
       <c r="C325">
         <f t="shared" si="6"/>
-        <v>4.1818046471737027</v>
+        <v>3.3530883260033879</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B326" s="3">
         <v>3</v>
       </c>
-      <c r="C326">
-        <f t="shared" si="6"/>
-        <v>3.730007725816376</v>
-      </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B327" s="4">
         <v>4</v>
-      </c>
-      <c r="C327">
-        <f>IF(0&lt;10^C296-10^(C$28*$B327+C$29),LOG(10^C296-10^(C$28*$B327+C$29)),0)</f>
-        <v>3.3245500520046676</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>